<commit_message>
Split analog SPI to be separate from SD pins, USB bus powered, added caps, updated todo, more
</commit_message>
<xml_diff>
--- a/data/ESP32.xlsx
+++ b/data/ESP32.xlsx
@@ -1278,7 +1278,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1293,10 +1293,6 @@
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1606,15 +1602,16 @@
   </sheetPr>
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S8" activeCellId="0" sqref="S8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M11" activeCellId="0" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="2" width="3.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="6.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="2" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="2" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="2" width="10.53"/>
@@ -1633,7 +1630,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="27" style="2" width="11.42"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>36</v>
       </c>
@@ -2336,7 +2333,7 @@
       <c r="P23" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="S23" s="4" t="s">
+      <c r="S23" s="2" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2473,71 +2470,71 @@
       <c r="A28" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="B28" s="5" t="n">
+      <c r="B28" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="G28" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="S28" s="6"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="B29" s="5" t="n">
+      <c r="B29" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="G29" s="5" t="s">
+      <c r="G29" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
-      <c r="Q29" s="5"/>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5" t="s">
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4" t="s">
         <v>236</v>
       </c>
     </row>
@@ -2545,40 +2542,40 @@
       <c r="A30" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="B30" s="5" t="n">
+      <c r="B30" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G30" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5" t="s">
+      <c r="H30" s="4"/>
+      <c r="I30" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
-      <c r="Q30" s="5"/>
-      <c r="R30" s="5" t="s">
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="S30" s="5" t="s">
+      <c r="S30" s="4" t="s">
         <v>243</v>
       </c>
     </row>
@@ -2586,40 +2583,40 @@
       <c r="A31" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B31" s="5" t="n">
+      <c r="B31" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G31" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5" t="s">
+      <c r="H31" s="4"/>
+      <c r="I31" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="5" t="s">
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="S31" s="5" t="s">
+      <c r="S31" s="4" t="s">
         <v>249</v>
       </c>
     </row>
@@ -2641,42 +2638,42 @@
       <c r="A33" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="B33" s="7" t="n">
+      <c r="B33" s="6" t="n">
         <v>20</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>252</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="7" t="s">
+      <c r="E33" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7" t="s">
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="M33" s="7" t="s">
+      <c r="M33" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="N33" s="7"/>
-      <c r="O33" s="7" t="s">
+      <c r="N33" s="6"/>
+      <c r="O33" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="P33" s="7"/>
-      <c r="Q33" s="7" t="s">
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="R33" s="7"/>
-      <c r="S33" s="7" t="s">
+      <c r="R33" s="6"/>
+      <c r="S33" s="6" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2684,40 +2681,40 @@
       <c r="A34" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B34" s="7" t="n">
+      <c r="B34" s="6" t="n">
         <v>19</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E34" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7" t="s">
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="M34" s="7" t="s">
+      <c r="M34" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="N34" s="7"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="7"/>
-      <c r="Q34" s="7" t="s">
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="R34" s="7"/>
-      <c r="S34" s="7" t="s">
+      <c r="R34" s="6"/>
+      <c r="S34" s="6" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2725,42 +2722,42 @@
       <c r="A35" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="B35" s="7" t="n">
+      <c r="B35" s="6" t="n">
         <v>22</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7" t="s">
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="M35" s="7" t="s">
+      <c r="M35" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="N35" s="7"/>
-      <c r="O35" s="7" t="s">
+      <c r="N35" s="6"/>
+      <c r="O35" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="P35" s="7"/>
-      <c r="Q35" s="7" t="s">
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="R35" s="7"/>
-      <c r="S35" s="7" t="s">
+      <c r="R35" s="6"/>
+      <c r="S35" s="6" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2768,42 +2765,42 @@
       <c r="A36" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="B36" s="7" t="n">
+      <c r="B36" s="6" t="n">
         <v>21</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E36" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7" t="s">
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6" t="s">
         <v>276</v>
       </c>
-      <c r="M36" s="7" t="s">
+      <c r="M36" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="N36" s="7"/>
-      <c r="O36" s="7" t="s">
+      <c r="N36" s="6"/>
+      <c r="O36" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="P36" s="7"/>
-      <c r="Q36" s="7" t="s">
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="R36" s="7"/>
-      <c r="S36" s="7" t="s">
+      <c r="R36" s="6"/>
+      <c r="S36" s="6" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2811,42 +2808,42 @@
       <c r="A37" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B37" s="7" t="n">
+      <c r="B37" s="6" t="n">
         <v>17</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E37" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7" t="s">
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="M37" s="7" t="s">
+      <c r="M37" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="N37" s="7"/>
-      <c r="O37" s="7" t="s">
+      <c r="N37" s="6"/>
+      <c r="O37" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="P37" s="7"/>
-      <c r="Q37" s="7" t="s">
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="R37" s="7"/>
-      <c r="S37" s="7" t="s">
+      <c r="R37" s="6"/>
+      <c r="S37" s="6" t="s">
         <v>259</v>
       </c>
     </row>
@@ -2854,42 +2851,42 @@
       <c r="A38" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="B38" s="7" t="n">
+      <c r="B38" s="6" t="n">
         <v>18</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7" t="s">
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="M38" s="7" t="s">
+      <c r="M38" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="N38" s="7"/>
-      <c r="O38" s="7" t="s">
+      <c r="N38" s="6"/>
+      <c r="O38" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="P38" s="7"/>
-      <c r="Q38" s="7" t="s">
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="R38" s="7"/>
-      <c r="S38" s="7" t="s">
+      <c r="R38" s="6"/>
+      <c r="S38" s="6" t="s">
         <v>259</v>
       </c>
     </row>

</xml_diff>